<commit_message>
Committing Login File Changes
Committing Login File Changes
</commit_message>
<xml_diff>
--- a/HayneedleScripts/Data/Login.xlsx
+++ b/HayneedleScripts/Data/Login.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ID</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Hayneedle1</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -380,19 +386,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +409,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -412,6 +422,9 @@
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login file and MyAccount test changes after revert
Trying my changes again after reverting the initial changes
</commit_message>
<xml_diff>
--- a/HayneedleScripts/Data/Login.xlsx
+++ b/HayneedleScripts/Data/Login.xlsx
@@ -36,7 +36,7 @@
     <t>Environment</t>
   </si>
   <si>
-    <t>test</t>
+    <t>stage</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>